<commit_message>
Update LoadData & WeatherData files
</commit_message>
<xml_diff>
--- a/NRI_STLF_Data/WeatherData/T_Tehran/T_tehran94.xlsx
+++ b/NRI_STLF_Data/WeatherData/T_Tehran/T_tehran94.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="7">
   <si>
     <t>Rain</t>
   </si>
@@ -379,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA365"/>
+  <dimension ref="A1:AA388"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A362" workbookViewId="0">
-      <selection activeCell="F366" sqref="F366:AC388"/>
+      <selection activeCell="C377" sqref="C377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -28643,6 +28643,1468 @@
       </c>
       <c r="AA365">
         <v>278</v>
+      </c>
+    </row>
+    <row r="366" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="F366">
+        <v>18</v>
+      </c>
+      <c r="G366">
+        <v>11</v>
+      </c>
+      <c r="H366">
+        <v>4</v>
+      </c>
+      <c r="I366">
+        <v>-1</v>
+      </c>
+      <c r="J366">
+        <v>-8</v>
+      </c>
+      <c r="K366">
+        <v>-11</v>
+      </c>
+      <c r="L366">
+        <v>39</v>
+      </c>
+      <c r="M366">
+        <v>24</v>
+      </c>
+      <c r="N366">
+        <v>6</v>
+      </c>
+      <c r="O366">
+        <v>1017</v>
+      </c>
+      <c r="P366">
+        <v>1014</v>
+      </c>
+      <c r="Q366">
+        <v>1011</v>
+      </c>
+      <c r="R366">
+        <v>14</v>
+      </c>
+      <c r="S366">
+        <v>10</v>
+      </c>
+      <c r="T366">
+        <v>10</v>
+      </c>
+      <c r="U366">
+        <v>37</v>
+      </c>
+      <c r="V366">
+        <v>21</v>
+      </c>
+      <c r="X366">
+        <v>0</v>
+      </c>
+      <c r="Y366">
+        <v>6</v>
+      </c>
+      <c r="AA366">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="367" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="F367">
+        <v>19</v>
+      </c>
+      <c r="G367">
+        <v>16</v>
+      </c>
+      <c r="H367">
+        <v>13</v>
+      </c>
+      <c r="I367">
+        <v>3</v>
+      </c>
+      <c r="J367">
+        <v>-1</v>
+      </c>
+      <c r="K367">
+        <v>-2</v>
+      </c>
+      <c r="L367">
+        <v>44</v>
+      </c>
+      <c r="M367">
+        <v>31</v>
+      </c>
+      <c r="N367">
+        <v>15</v>
+      </c>
+      <c r="O367">
+        <v>1016</v>
+      </c>
+      <c r="P367">
+        <v>1013</v>
+      </c>
+      <c r="Q367">
+        <v>1007</v>
+      </c>
+      <c r="R367">
+        <v>10</v>
+      </c>
+      <c r="S367">
+        <v>10</v>
+      </c>
+      <c r="T367">
+        <v>10</v>
+      </c>
+      <c r="U367">
+        <v>29</v>
+      </c>
+      <c r="V367">
+        <v>10</v>
+      </c>
+      <c r="X367">
+        <v>0</v>
+      </c>
+      <c r="Y367">
+        <v>5</v>
+      </c>
+      <c r="Z367" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA367">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="368" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="F368">
+        <v>16</v>
+      </c>
+      <c r="G368">
+        <v>12</v>
+      </c>
+      <c r="H368">
+        <v>8</v>
+      </c>
+      <c r="I368">
+        <v>6</v>
+      </c>
+      <c r="J368">
+        <v>4</v>
+      </c>
+      <c r="K368">
+        <v>1</v>
+      </c>
+      <c r="L368">
+        <v>82</v>
+      </c>
+      <c r="M368">
+        <v>63</v>
+      </c>
+      <c r="N368">
+        <v>34</v>
+      </c>
+      <c r="O368">
+        <v>1013</v>
+      </c>
+      <c r="P368">
+        <v>1011</v>
+      </c>
+      <c r="Q368">
+        <v>1004</v>
+      </c>
+      <c r="R368">
+        <v>10</v>
+      </c>
+      <c r="S368">
+        <v>9</v>
+      </c>
+      <c r="T368">
+        <v>3</v>
+      </c>
+      <c r="U368">
+        <v>55</v>
+      </c>
+      <c r="V368">
+        <v>16</v>
+      </c>
+      <c r="X368">
+        <v>8.89</v>
+      </c>
+      <c r="Y368">
+        <v>5</v>
+      </c>
+      <c r="Z368" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA368">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="369" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F369">
+        <v>15</v>
+      </c>
+      <c r="G369">
+        <v>9</v>
+      </c>
+      <c r="H369">
+        <v>3</v>
+      </c>
+      <c r="I369">
+        <v>4</v>
+      </c>
+      <c r="J369">
+        <v>-2</v>
+      </c>
+      <c r="K369">
+        <v>-11</v>
+      </c>
+      <c r="L369">
+        <v>81</v>
+      </c>
+      <c r="M369">
+        <v>46</v>
+      </c>
+      <c r="N369">
+        <v>9</v>
+      </c>
+      <c r="O369">
+        <v>1015</v>
+      </c>
+      <c r="P369">
+        <v>1012</v>
+      </c>
+      <c r="Q369">
+        <v>1009</v>
+      </c>
+      <c r="R369">
+        <v>14</v>
+      </c>
+      <c r="S369">
+        <v>10</v>
+      </c>
+      <c r="T369">
+        <v>8</v>
+      </c>
+      <c r="U369">
+        <v>48</v>
+      </c>
+      <c r="V369">
+        <v>26</v>
+      </c>
+      <c r="X369">
+        <v>0</v>
+      </c>
+      <c r="Y369">
+        <v>1</v>
+      </c>
+      <c r="AA369">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="370" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F370">
+        <v>19</v>
+      </c>
+      <c r="G370">
+        <v>12</v>
+      </c>
+      <c r="H370">
+        <v>6</v>
+      </c>
+      <c r="I370">
+        <v>-2</v>
+      </c>
+      <c r="J370">
+        <v>-5</v>
+      </c>
+      <c r="K370">
+        <v>-8</v>
+      </c>
+      <c r="L370">
+        <v>53</v>
+      </c>
+      <c r="M370">
+        <v>30</v>
+      </c>
+      <c r="N370">
+        <v>8</v>
+      </c>
+      <c r="O370">
+        <v>1021</v>
+      </c>
+      <c r="P370">
+        <v>1019</v>
+      </c>
+      <c r="Q370">
+        <v>1015</v>
+      </c>
+      <c r="R370">
+        <v>11</v>
+      </c>
+      <c r="S370">
+        <v>10</v>
+      </c>
+      <c r="T370">
+        <v>10</v>
+      </c>
+      <c r="U370">
+        <v>23</v>
+      </c>
+      <c r="V370">
+        <v>10</v>
+      </c>
+      <c r="X370">
+        <v>0</v>
+      </c>
+      <c r="Y370">
+        <v>6</v>
+      </c>
+      <c r="AA370">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="371" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F371">
+        <v>21</v>
+      </c>
+      <c r="G371">
+        <v>16</v>
+      </c>
+      <c r="H371">
+        <v>9</v>
+      </c>
+      <c r="I371">
+        <v>0</v>
+      </c>
+      <c r="J371">
+        <v>-4</v>
+      </c>
+      <c r="K371">
+        <v>-10</v>
+      </c>
+      <c r="L371">
+        <v>44</v>
+      </c>
+      <c r="M371">
+        <v>25</v>
+      </c>
+      <c r="N371">
+        <v>6</v>
+      </c>
+      <c r="O371">
+        <v>1022</v>
+      </c>
+      <c r="P371">
+        <v>1019</v>
+      </c>
+      <c r="Q371">
+        <v>1013</v>
+      </c>
+      <c r="R371">
+        <v>10</v>
+      </c>
+      <c r="S371">
+        <v>10</v>
+      </c>
+      <c r="T371">
+        <v>10</v>
+      </c>
+      <c r="U371">
+        <v>29</v>
+      </c>
+      <c r="V371">
+        <v>8</v>
+      </c>
+      <c r="X371">
+        <v>0</v>
+      </c>
+      <c r="Y371">
+        <v>5</v>
+      </c>
+      <c r="AA371">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="372" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F372">
+        <v>18</v>
+      </c>
+      <c r="G372">
+        <v>14</v>
+      </c>
+      <c r="H372">
+        <v>11</v>
+      </c>
+      <c r="I372">
+        <v>8</v>
+      </c>
+      <c r="J372">
+        <v>3</v>
+      </c>
+      <c r="K372">
+        <v>-4</v>
+      </c>
+      <c r="L372">
+        <v>77</v>
+      </c>
+      <c r="M372">
+        <v>49</v>
+      </c>
+      <c r="N372">
+        <v>11</v>
+      </c>
+      <c r="O372">
+        <v>1021</v>
+      </c>
+      <c r="P372">
+        <v>1018</v>
+      </c>
+      <c r="Q372">
+        <v>1013</v>
+      </c>
+      <c r="R372">
+        <v>10</v>
+      </c>
+      <c r="S372">
+        <v>8</v>
+      </c>
+      <c r="T372">
+        <v>6</v>
+      </c>
+      <c r="U372">
+        <v>34</v>
+      </c>
+      <c r="V372">
+        <v>10</v>
+      </c>
+      <c r="X372">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="Y372">
+        <v>7</v>
+      </c>
+      <c r="Z372" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA372">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="373" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F373">
+        <v>14</v>
+      </c>
+      <c r="G373">
+        <v>12</v>
+      </c>
+      <c r="H373">
+        <v>10</v>
+      </c>
+      <c r="I373">
+        <v>9</v>
+      </c>
+      <c r="J373">
+        <v>8</v>
+      </c>
+      <c r="K373">
+        <v>7</v>
+      </c>
+      <c r="L373">
+        <v>88</v>
+      </c>
+      <c r="M373">
+        <v>73</v>
+      </c>
+      <c r="N373">
+        <v>52</v>
+      </c>
+      <c r="O373">
+        <v>1018</v>
+      </c>
+      <c r="P373">
+        <v>1013</v>
+      </c>
+      <c r="Q373">
+        <v>1007</v>
+      </c>
+      <c r="R373">
+        <v>11</v>
+      </c>
+      <c r="S373">
+        <v>8</v>
+      </c>
+      <c r="T373">
+        <v>3</v>
+      </c>
+      <c r="U373">
+        <v>19</v>
+      </c>
+      <c r="V373">
+        <v>10</v>
+      </c>
+      <c r="X373">
+        <v>3.05</v>
+      </c>
+      <c r="Y373">
+        <v>8</v>
+      </c>
+      <c r="Z373" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA373">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="374" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F374">
+        <v>21</v>
+      </c>
+      <c r="G374">
+        <v>16</v>
+      </c>
+      <c r="H374">
+        <v>10</v>
+      </c>
+      <c r="I374">
+        <v>8</v>
+      </c>
+      <c r="J374">
+        <v>4</v>
+      </c>
+      <c r="K374">
+        <v>-2</v>
+      </c>
+      <c r="L374">
+        <v>82</v>
+      </c>
+      <c r="M374">
+        <v>48</v>
+      </c>
+      <c r="N374">
+        <v>15</v>
+      </c>
+      <c r="O374">
+        <v>1012</v>
+      </c>
+      <c r="P374">
+        <v>1009</v>
+      </c>
+      <c r="Q374">
+        <v>1003</v>
+      </c>
+      <c r="R374">
+        <v>10</v>
+      </c>
+      <c r="S374">
+        <v>10</v>
+      </c>
+      <c r="T374">
+        <v>8</v>
+      </c>
+      <c r="U374">
+        <v>34</v>
+      </c>
+      <c r="V374">
+        <v>14</v>
+      </c>
+      <c r="X374">
+        <v>0.25</v>
+      </c>
+      <c r="Y374">
+        <v>4</v>
+      </c>
+      <c r="Z374" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA374">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="375" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F375">
+        <v>19</v>
+      </c>
+      <c r="G375">
+        <v>15</v>
+      </c>
+      <c r="H375">
+        <v>11</v>
+      </c>
+      <c r="I375">
+        <v>7</v>
+      </c>
+      <c r="J375">
+        <v>-2</v>
+      </c>
+      <c r="K375">
+        <v>-11</v>
+      </c>
+      <c r="L375">
+        <v>76</v>
+      </c>
+      <c r="M375">
+        <v>33</v>
+      </c>
+      <c r="N375">
+        <v>6</v>
+      </c>
+      <c r="O375">
+        <v>1010</v>
+      </c>
+      <c r="P375">
+        <v>1008</v>
+      </c>
+      <c r="Q375">
+        <v>1001</v>
+      </c>
+      <c r="R375">
+        <v>14</v>
+      </c>
+      <c r="S375">
+        <v>10</v>
+      </c>
+      <c r="T375">
+        <v>7</v>
+      </c>
+      <c r="U375">
+        <v>37</v>
+      </c>
+      <c r="V375">
+        <v>19</v>
+      </c>
+      <c r="X375">
+        <v>0.25</v>
+      </c>
+      <c r="Y375">
+        <v>4</v>
+      </c>
+      <c r="Z375" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA375">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="376" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F376">
+        <v>15</v>
+      </c>
+      <c r="G376">
+        <v>12</v>
+      </c>
+      <c r="H376">
+        <v>9</v>
+      </c>
+      <c r="I376">
+        <v>-4</v>
+      </c>
+      <c r="J376">
+        <v>-7</v>
+      </c>
+      <c r="K376">
+        <v>-12</v>
+      </c>
+      <c r="L376">
+        <v>35</v>
+      </c>
+      <c r="M376">
+        <v>25</v>
+      </c>
+      <c r="N376">
+        <v>7</v>
+      </c>
+      <c r="O376">
+        <v>1015</v>
+      </c>
+      <c r="P376">
+        <v>1013</v>
+      </c>
+      <c r="Q376">
+        <v>1006</v>
+      </c>
+      <c r="R376">
+        <v>14</v>
+      </c>
+      <c r="S376">
+        <v>11</v>
+      </c>
+      <c r="T376">
+        <v>10</v>
+      </c>
+      <c r="U376">
+        <v>55</v>
+      </c>
+      <c r="V376">
+        <v>29</v>
+      </c>
+      <c r="X376">
+        <v>0</v>
+      </c>
+      <c r="Y376">
+        <v>1</v>
+      </c>
+      <c r="AA376">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="377" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F377">
+        <v>17</v>
+      </c>
+      <c r="G377">
+        <v>11</v>
+      </c>
+      <c r="H377">
+        <v>6</v>
+      </c>
+      <c r="I377">
+        <v>-1</v>
+      </c>
+      <c r="J377">
+        <v>-7</v>
+      </c>
+      <c r="K377">
+        <v>-12</v>
+      </c>
+      <c r="L377">
+        <v>46</v>
+      </c>
+      <c r="M377">
+        <v>28</v>
+      </c>
+      <c r="N377">
+        <v>6</v>
+      </c>
+      <c r="O377">
+        <v>1018</v>
+      </c>
+      <c r="P377">
+        <v>1014</v>
+      </c>
+      <c r="Q377">
+        <v>1010</v>
+      </c>
+      <c r="R377">
+        <v>11</v>
+      </c>
+      <c r="S377">
+        <v>10</v>
+      </c>
+      <c r="T377">
+        <v>10</v>
+      </c>
+      <c r="U377">
+        <v>26</v>
+      </c>
+      <c r="V377">
+        <v>10</v>
+      </c>
+      <c r="X377">
+        <v>0</v>
+      </c>
+      <c r="Y377">
+        <v>4</v>
+      </c>
+      <c r="AA377">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="378" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F378">
+        <v>7</v>
+      </c>
+      <c r="G378">
+        <v>6</v>
+      </c>
+      <c r="H378">
+        <v>5</v>
+      </c>
+      <c r="I378">
+        <v>4</v>
+      </c>
+      <c r="J378">
+        <v>2</v>
+      </c>
+      <c r="K378">
+        <v>-3</v>
+      </c>
+      <c r="L378">
+        <v>87</v>
+      </c>
+      <c r="M378">
+        <v>71</v>
+      </c>
+      <c r="N378">
+        <v>33</v>
+      </c>
+      <c r="O378">
+        <v>1021</v>
+      </c>
+      <c r="P378">
+        <v>1016</v>
+      </c>
+      <c r="Q378">
+        <v>1011</v>
+      </c>
+      <c r="R378">
+        <v>10</v>
+      </c>
+      <c r="S378">
+        <v>8</v>
+      </c>
+      <c r="T378">
+        <v>3</v>
+      </c>
+      <c r="U378">
+        <v>26</v>
+      </c>
+      <c r="V378">
+        <v>16</v>
+      </c>
+      <c r="X378">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="Y378">
+        <v>7</v>
+      </c>
+      <c r="Z378" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA378">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="379" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F379">
+        <v>14</v>
+      </c>
+      <c r="G379">
+        <v>8</v>
+      </c>
+      <c r="H379">
+        <v>2</v>
+      </c>
+      <c r="I379">
+        <v>1</v>
+      </c>
+      <c r="J379">
+        <v>-3</v>
+      </c>
+      <c r="K379">
+        <v>-6</v>
+      </c>
+      <c r="L379">
+        <v>81</v>
+      </c>
+      <c r="M379">
+        <v>47</v>
+      </c>
+      <c r="N379">
+        <v>14</v>
+      </c>
+      <c r="O379">
+        <v>1021</v>
+      </c>
+      <c r="P379">
+        <v>1018</v>
+      </c>
+      <c r="Q379">
+        <v>1016</v>
+      </c>
+      <c r="R379">
+        <v>14</v>
+      </c>
+      <c r="S379">
+        <v>10</v>
+      </c>
+      <c r="T379">
+        <v>10</v>
+      </c>
+      <c r="U379">
+        <v>34</v>
+      </c>
+      <c r="V379">
+        <v>14</v>
+      </c>
+      <c r="X379">
+        <v>0</v>
+      </c>
+      <c r="Y379">
+        <v>2</v>
+      </c>
+      <c r="AA379">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="380" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F380">
+        <v>18</v>
+      </c>
+      <c r="G380">
+        <v>12</v>
+      </c>
+      <c r="H380">
+        <v>6</v>
+      </c>
+      <c r="I380">
+        <v>-2</v>
+      </c>
+      <c r="J380">
+        <v>-7</v>
+      </c>
+      <c r="K380">
+        <v>-15</v>
+      </c>
+      <c r="L380">
+        <v>57</v>
+      </c>
+      <c r="M380">
+        <v>28</v>
+      </c>
+      <c r="N380">
+        <v>5</v>
+      </c>
+      <c r="O380">
+        <v>1018</v>
+      </c>
+      <c r="P380">
+        <v>1016</v>
+      </c>
+      <c r="Q380">
+        <v>1012</v>
+      </c>
+      <c r="R380">
+        <v>14</v>
+      </c>
+      <c r="S380">
+        <v>10</v>
+      </c>
+      <c r="T380">
+        <v>10</v>
+      </c>
+      <c r="U380">
+        <v>19</v>
+      </c>
+      <c r="V380">
+        <v>6</v>
+      </c>
+      <c r="X380">
+        <v>0</v>
+      </c>
+      <c r="Y380">
+        <v>4</v>
+      </c>
+      <c r="AA380">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="381" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F381">
+        <v>19</v>
+      </c>
+      <c r="G381">
+        <v>14</v>
+      </c>
+      <c r="H381">
+        <v>11</v>
+      </c>
+      <c r="I381">
+        <v>2</v>
+      </c>
+      <c r="J381">
+        <v>-3</v>
+      </c>
+      <c r="K381">
+        <v>-7</v>
+      </c>
+      <c r="L381">
+        <v>54</v>
+      </c>
+      <c r="M381">
+        <v>29</v>
+      </c>
+      <c r="N381">
+        <v>12</v>
+      </c>
+      <c r="O381">
+        <v>1015</v>
+      </c>
+      <c r="P381">
+        <v>1014</v>
+      </c>
+      <c r="Q381">
+        <v>1008</v>
+      </c>
+      <c r="R381">
+        <v>14</v>
+      </c>
+      <c r="S381">
+        <v>10</v>
+      </c>
+      <c r="T381">
+        <v>10</v>
+      </c>
+      <c r="U381">
+        <v>48</v>
+      </c>
+      <c r="V381">
+        <v>18</v>
+      </c>
+      <c r="W381">
+        <v>55</v>
+      </c>
+      <c r="X381">
+        <v>0</v>
+      </c>
+      <c r="Y381">
+        <v>3</v>
+      </c>
+      <c r="AA381">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="382" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F382">
+        <v>21</v>
+      </c>
+      <c r="G382">
+        <v>15</v>
+      </c>
+      <c r="H382">
+        <v>9</v>
+      </c>
+      <c r="I382">
+        <v>7</v>
+      </c>
+      <c r="J382">
+        <v>-3</v>
+      </c>
+      <c r="K382">
+        <v>-9</v>
+      </c>
+      <c r="L382">
+        <v>68</v>
+      </c>
+      <c r="M382">
+        <v>30</v>
+      </c>
+      <c r="N382">
+        <v>8</v>
+      </c>
+      <c r="O382">
+        <v>1015</v>
+      </c>
+      <c r="P382">
+        <v>1013</v>
+      </c>
+      <c r="Q382">
+        <v>1008</v>
+      </c>
+      <c r="R382">
+        <v>14</v>
+      </c>
+      <c r="S382">
+        <v>10</v>
+      </c>
+      <c r="T382">
+        <v>10</v>
+      </c>
+      <c r="U382">
+        <v>37</v>
+      </c>
+      <c r="V382">
+        <v>19</v>
+      </c>
+      <c r="X382">
+        <v>0</v>
+      </c>
+      <c r="Y382">
+        <v>2</v>
+      </c>
+      <c r="AA382">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="383" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F383">
+        <v>22</v>
+      </c>
+      <c r="G383">
+        <v>17</v>
+      </c>
+      <c r="H383">
+        <v>11</v>
+      </c>
+      <c r="I383">
+        <v>0</v>
+      </c>
+      <c r="J383">
+        <v>-4</v>
+      </c>
+      <c r="K383">
+        <v>-8</v>
+      </c>
+      <c r="L383">
+        <v>44</v>
+      </c>
+      <c r="M383">
+        <v>23</v>
+      </c>
+      <c r="N383">
+        <v>7</v>
+      </c>
+      <c r="O383">
+        <v>1016</v>
+      </c>
+      <c r="P383">
+        <v>1013</v>
+      </c>
+      <c r="Q383">
+        <v>1008</v>
+      </c>
+      <c r="R383">
+        <v>11</v>
+      </c>
+      <c r="S383">
+        <v>10</v>
+      </c>
+      <c r="T383">
+        <v>8</v>
+      </c>
+      <c r="U383">
+        <v>19</v>
+      </c>
+      <c r="V383">
+        <v>10</v>
+      </c>
+      <c r="X383">
+        <v>0</v>
+      </c>
+      <c r="Y383">
+        <v>1</v>
+      </c>
+      <c r="AA383">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="384" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F384">
+        <v>24</v>
+      </c>
+      <c r="G384">
+        <v>18</v>
+      </c>
+      <c r="H384">
+        <v>12</v>
+      </c>
+      <c r="I384">
+        <v>-3</v>
+      </c>
+      <c r="J384">
+        <v>-6</v>
+      </c>
+      <c r="K384">
+        <v>-11</v>
+      </c>
+      <c r="L384">
+        <v>33</v>
+      </c>
+      <c r="M384">
+        <v>18</v>
+      </c>
+      <c r="N384">
+        <v>4</v>
+      </c>
+      <c r="O384">
+        <v>1016</v>
+      </c>
+      <c r="P384">
+        <v>1013</v>
+      </c>
+      <c r="Q384">
+        <v>1007</v>
+      </c>
+      <c r="R384">
+        <v>11</v>
+      </c>
+      <c r="S384">
+        <v>10</v>
+      </c>
+      <c r="T384">
+        <v>10</v>
+      </c>
+      <c r="U384">
+        <v>37</v>
+      </c>
+      <c r="V384">
+        <v>11</v>
+      </c>
+      <c r="X384">
+        <v>0</v>
+      </c>
+      <c r="Y384">
+        <v>1</v>
+      </c>
+      <c r="AA384">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="385" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F385">
+        <v>23</v>
+      </c>
+      <c r="G385">
+        <v>17</v>
+      </c>
+      <c r="H385">
+        <v>10</v>
+      </c>
+      <c r="I385">
+        <v>3</v>
+      </c>
+      <c r="J385">
+        <v>-2</v>
+      </c>
+      <c r="K385">
+        <v>-5</v>
+      </c>
+      <c r="L385">
+        <v>45</v>
+      </c>
+      <c r="M385">
+        <v>27</v>
+      </c>
+      <c r="N385">
+        <v>8</v>
+      </c>
+      <c r="O385">
+        <v>1018</v>
+      </c>
+      <c r="P385">
+        <v>1015</v>
+      </c>
+      <c r="Q385">
+        <v>1009</v>
+      </c>
+      <c r="R385">
+        <v>11</v>
+      </c>
+      <c r="S385">
+        <v>10</v>
+      </c>
+      <c r="T385">
+        <v>10</v>
+      </c>
+      <c r="U385">
+        <v>19</v>
+      </c>
+      <c r="V385">
+        <v>8</v>
+      </c>
+      <c r="W385">
+        <v>37</v>
+      </c>
+      <c r="X385">
+        <v>0</v>
+      </c>
+      <c r="Y385">
+        <v>3</v>
+      </c>
+      <c r="AA385">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="386" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F386">
+        <v>20</v>
+      </c>
+      <c r="G386">
+        <v>16</v>
+      </c>
+      <c r="H386">
+        <v>11</v>
+      </c>
+      <c r="I386">
+        <v>7</v>
+      </c>
+      <c r="J386">
+        <v>3</v>
+      </c>
+      <c r="K386">
+        <v>0</v>
+      </c>
+      <c r="L386">
+        <v>72</v>
+      </c>
+      <c r="M386">
+        <v>40</v>
+      </c>
+      <c r="N386">
+        <v>21</v>
+      </c>
+      <c r="O386">
+        <v>1019</v>
+      </c>
+      <c r="P386">
+        <v>1016</v>
+      </c>
+      <c r="Q386">
+        <v>1011</v>
+      </c>
+      <c r="R386">
+        <v>10</v>
+      </c>
+      <c r="S386">
+        <v>10</v>
+      </c>
+      <c r="T386">
+        <v>7</v>
+      </c>
+      <c r="U386">
+        <v>23</v>
+      </c>
+      <c r="V386">
+        <v>10</v>
+      </c>
+      <c r="X386">
+        <v>1.02</v>
+      </c>
+      <c r="Y386">
+        <v>4</v>
+      </c>
+      <c r="Z386" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA386">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="387" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F387">
+        <v>23</v>
+      </c>
+      <c r="G387">
+        <v>18</v>
+      </c>
+      <c r="H387">
+        <v>12</v>
+      </c>
+      <c r="I387">
+        <v>10</v>
+      </c>
+      <c r="J387">
+        <v>3</v>
+      </c>
+      <c r="K387">
+        <v>-1</v>
+      </c>
+      <c r="L387">
+        <v>68</v>
+      </c>
+      <c r="M387">
+        <v>37</v>
+      </c>
+      <c r="N387">
+        <v>15</v>
+      </c>
+      <c r="O387">
+        <v>1019</v>
+      </c>
+      <c r="P387">
+        <v>1017</v>
+      </c>
+      <c r="Q387">
+        <v>1011</v>
+      </c>
+      <c r="R387">
+        <v>10</v>
+      </c>
+      <c r="S387">
+        <v>10</v>
+      </c>
+      <c r="T387">
+        <v>10</v>
+      </c>
+      <c r="U387">
+        <v>34</v>
+      </c>
+      <c r="V387">
+        <v>8</v>
+      </c>
+      <c r="X387">
+        <v>0</v>
+      </c>
+      <c r="Y387">
+        <v>4</v>
+      </c>
+      <c r="Z387" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA387">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="388" spans="6:27" x14ac:dyDescent="0.2">
+      <c r="F388">
+        <v>23</v>
+      </c>
+      <c r="G388">
+        <v>17</v>
+      </c>
+      <c r="H388">
+        <v>11</v>
+      </c>
+      <c r="I388">
+        <v>10</v>
+      </c>
+      <c r="J388">
+        <v>7</v>
+      </c>
+      <c r="K388">
+        <v>2</v>
+      </c>
+      <c r="L388">
+        <v>82</v>
+      </c>
+      <c r="M388">
+        <v>56</v>
+      </c>
+      <c r="N388">
+        <v>17</v>
+      </c>
+      <c r="O388">
+        <v>1017</v>
+      </c>
+      <c r="P388">
+        <v>1015</v>
+      </c>
+      <c r="Q388">
+        <v>1009</v>
+      </c>
+      <c r="R388">
+        <v>10</v>
+      </c>
+      <c r="S388">
+        <v>8</v>
+      </c>
+      <c r="T388">
+        <v>3</v>
+      </c>
+      <c r="U388">
+        <v>40</v>
+      </c>
+      <c r="V388">
+        <v>16</v>
+      </c>
+      <c r="X388">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="Y388">
+        <v>6</v>
+      </c>
+      <c r="Z388" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA388">
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>